<commit_message>
Update Wen & Thu Schedule
</commit_message>
<xml_diff>
--- a/resources/schedule/schedule-summer-camp.xlsx
+++ b/resources/schedule/schedule-summer-camp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="204">
   <si>
     <t>city-experience</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1027,59 +1027,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finish experience prototypes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>09:50-10:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10:30-11:15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11:15-11:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Write up what you learned</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11:30-12:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tools (Sketch, Modao)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12:30-13:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13:30-14:15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Low-Fi Prototype Lecture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14:15-16:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Build 1 Low-Fi Prototype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>16:00-17:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17:00-17:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1090,6 +1046,106 @@
     <t>Test with 3 users
 45 - test
 15 - report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>09:30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue Light"/>
+      </rPr>
+      <t>-10:15</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:15-12:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:30-13:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:15-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:30-15:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30-15:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:45-17:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:15-18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-12:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:20-12:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish experience prototypes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 tests &amp; Finish experience prototypes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:45-14:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:10-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wrap-up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:30-15:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low-Fi Prototype Lecture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:10-16:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build one Low-Fi Prototype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:40-17:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:40-18:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1097,7 +1153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1192,6 +1248,12 @@
       <name val="Helvetica Neue"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1294,7 +1356,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1420,6 +1482,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1737,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="138" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
@@ -2100,7 +2165,7 @@
         <v>177</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2113,7 +2178,7 @@
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>39</v>
@@ -2132,10 +2197,10 @@
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="3" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>36</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2148,10 +2213,10 @@
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="3" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2163,11 +2228,11 @@
         <v>11</v>
       </c>
       <c r="F29" s="35"/>
-      <c r="G29" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>184</v>
+      <c r="G29" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2179,11 +2244,11 @@
         <v>78</v>
       </c>
       <c r="F30" s="35"/>
-      <c r="G30" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>11</v>
+      <c r="G30" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45">
@@ -2196,10 +2261,10 @@
       </c>
       <c r="F31" s="35"/>
       <c r="G31" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>187</v>
+        <v>198</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2212,10 +2277,10 @@
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>189</v>
+        <v>200</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60">
@@ -2228,10 +2293,10 @@
       </c>
       <c r="F33" s="35"/>
       <c r="G33" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2240,10 +2305,10 @@
       <c r="C34" s="36"/>
       <c r="F34" s="35"/>
       <c r="G34" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>192</v>
+        <v>203</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2259,6 +2324,10 @@
       </c>
       <c r="C36" s="34"/>
       <c r="F36" s="35"/>
+      <c r="G36" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="33"/>
@@ -2269,6 +2338,12 @@
         <v>57</v>
       </c>
       <c r="F37" s="35"/>
+      <c r="G37" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="33"/>
@@ -2279,6 +2354,12 @@
         <v>11</v>
       </c>
       <c r="F38" s="35"/>
+      <c r="G38" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="33"/>
@@ -2289,6 +2370,12 @@
         <v>58</v>
       </c>
       <c r="F39" s="35"/>
+      <c r="G39" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="33"/>
@@ -2299,6 +2386,12 @@
         <v>59</v>
       </c>
       <c r="F40" s="35"/>
+      <c r="G40" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="33"/>
@@ -2309,6 +2402,12 @@
         <v>60</v>
       </c>
       <c r="F41" s="35"/>
+      <c r="G41" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="33"/>
@@ -2319,6 +2418,12 @@
         <v>61</v>
       </c>
       <c r="F42" s="35"/>
+      <c r="G42" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="33"/>
@@ -2329,12 +2434,24 @@
         <v>62</v>
       </c>
       <c r="F43" s="35"/>
+      <c r="G43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="33"/>
       <c r="B44" s="37"/>
       <c r="C44" s="36"/>
       <c r="F44" s="35"/>
+      <c r="G44" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="33"/>
@@ -2431,7 +2548,8 @@
       <c r="F54" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A54"/>
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
schedule & pdf updated
</commit_message>
<xml_diff>
--- a/resources/schedule/schedule-summer-camp.xlsx
+++ b/resources/schedule/schedule-summer-camp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\viax-summer-2018\resources\schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glorialiu/Documents/GitHub/viax-summer-2018/resources/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3C17A913-2061-E846-B424-C4A2AE3A460F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="28800" windowHeight="16164"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCHEDULE" sheetId="2" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="199">
   <si>
     <t>city-experience</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1027,59 +1028,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finish experience prototypes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>09:50-10:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10:30-11:15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11:15-11:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write up what you learned</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11:30-12:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tools (Sketch, Modao)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>12:30-13:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13:30-14:15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Low-Fi Prototype Lecture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14:15-16:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Build 1 Low-Fi Prototype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>16:00-17:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17:00-17:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1090,14 +1047,88 @@
     <t>Test with 3 users
 45 - test
 15 - report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-12:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 tests &amp; Finish experience prototypes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:20-12:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:45-14:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:10-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wrap-up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:30-15:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:10-16:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build one Low-Fi Prototype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:40-17:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:40-18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30-15:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:45-17:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:15-18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>09:30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue Light"/>
+      </rPr>
+      <t>-10:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00-12:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1192,6 +1223,12 @@
       <name val="Helvetica Neue"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1294,7 +1331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1420,6 +1457,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1734,26 +1774,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="138" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="175" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.81640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.81640625" style="36"/>
-    <col min="6" max="6" width="1.81640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="40.81640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.81640625" style="3"/>
+    <col min="1" max="1" width="1.83203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="36"/>
+    <col min="6" max="6" width="1.83203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="64.05" customHeight="1">
+    <row r="1" spans="1:8" ht="64" customHeight="1">
       <c r="A1" s="33">
         <v>1</v>
       </c>
@@ -1925,7 +1965,7 @@
       <c r="C12" s="36"/>
       <c r="F12" s="35"/>
     </row>
-    <row r="13" spans="1:8" ht="64.05" customHeight="1">
+    <row r="13" spans="1:8" ht="64" customHeight="1">
       <c r="A13" s="33"/>
       <c r="B13" s="34" t="s">
         <v>22</v>
@@ -2059,7 +2099,7 @@
       <c r="C22" s="36"/>
       <c r="F22" s="35"/>
     </row>
-    <row r="23" spans="1:9" ht="64.05" customHeight="1">
+    <row r="23" spans="1:9" ht="64" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="34" t="s">
         <v>33</v>
@@ -2100,7 +2140,7 @@
         <v>177</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2113,7 +2153,7 @@
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>39</v>
@@ -2132,10 +2172,10 @@
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>36</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2148,10 +2188,10 @@
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>182</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2163,11 +2203,11 @@
         <v>11</v>
       </c>
       <c r="F29" s="35"/>
-      <c r="G29" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>184</v>
+      <c r="G29" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2179,14 +2219,14 @@
         <v>78</v>
       </c>
       <c r="F30" s="35"/>
-      <c r="G30" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="45">
+      <c r="G30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="48">
       <c r="A31" s="33"/>
       <c r="B31" s="3" t="s">
         <v>47</v>
@@ -2196,10 +2236,10 @@
       </c>
       <c r="F31" s="35"/>
       <c r="G31" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2212,13 +2252,13 @@
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60">
+        <v>190</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="64">
       <c r="A33" s="33"/>
       <c r="B33" s="3" t="s">
         <v>49</v>
@@ -2228,10 +2268,10 @@
       </c>
       <c r="F33" s="35"/>
       <c r="G33" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2240,10 +2280,10 @@
       <c r="C34" s="36"/>
       <c r="F34" s="35"/>
       <c r="G34" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2252,13 +2292,17 @@
       <c r="C35" s="36"/>
       <c r="F35" s="35"/>
     </row>
-    <row r="36" spans="1:8" ht="64.05" customHeight="1">
+    <row r="36" spans="1:8" ht="64" customHeight="1">
       <c r="A36" s="33"/>
       <c r="B36" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C36" s="34"/>
       <c r="F36" s="35"/>
+      <c r="G36" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="33"/>
@@ -2269,6 +2313,12 @@
         <v>57</v>
       </c>
       <c r="F37" s="35"/>
+      <c r="G37" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="33"/>
@@ -2279,6 +2329,12 @@
         <v>11</v>
       </c>
       <c r="F38" s="35"/>
+      <c r="G38" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="33"/>
@@ -2289,6 +2345,12 @@
         <v>58</v>
       </c>
       <c r="F39" s="35"/>
+      <c r="G39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="33"/>
@@ -2299,6 +2361,12 @@
         <v>59</v>
       </c>
       <c r="F40" s="35"/>
+      <c r="G40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="33"/>
@@ -2309,6 +2377,12 @@
         <v>60</v>
       </c>
       <c r="F41" s="35"/>
+      <c r="G41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="33"/>
@@ -2319,6 +2393,12 @@
         <v>61</v>
       </c>
       <c r="F42" s="35"/>
+      <c r="G42" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="33"/>
@@ -2329,12 +2409,24 @@
         <v>62</v>
       </c>
       <c r="F43" s="35"/>
+      <c r="G43" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="33"/>
       <c r="B44" s="37"/>
       <c r="C44" s="36"/>
       <c r="F44" s="35"/>
+      <c r="G44" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="33"/>
@@ -2342,7 +2434,7 @@
       <c r="C45" s="36"/>
       <c r="F45" s="35"/>
     </row>
-    <row r="46" spans="1:8" ht="64.05" customHeight="1">
+    <row r="46" spans="1:8" ht="64" customHeight="1">
       <c r="A46" s="33"/>
       <c r="B46" s="34" t="s">
         <v>63</v>
@@ -2390,7 +2482,7 @@
       </c>
       <c r="F50" s="35"/>
     </row>
-    <row r="51" spans="1:6" ht="30">
+    <row r="51" spans="1:6" ht="32">
       <c r="A51" s="33"/>
       <c r="B51" s="3" t="s">
         <v>74</v>
@@ -2431,7 +2523,8 @@
       <c r="F54" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A54"/>
     <mergeCell ref="B1:C1"/>
@@ -2456,24 +2549,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="106" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="60.81640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" style="28" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="10.81640625" style="11"/>
+    <col min="3" max="3" width="10.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
@@ -2502,7 +2595,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45.6">
+    <row r="2" spans="1:8" ht="47">
       <c r="A2" s="29" t="s">
         <v>131</v>
       </c>
@@ -2526,7 +2619,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45.6">
+    <row r="3" spans="1:8" ht="47">
       <c r="A3" s="16" t="s">
         <v>125</v>
       </c>
@@ -2552,7 +2645,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45.6">
+    <row r="4" spans="1:8" ht="47">
       <c r="A4" s="16" t="s">
         <v>127</v>
       </c>
@@ -2576,7 +2669,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30.6">
+    <row r="5" spans="1:8" ht="31">
       <c r="A5" s="19" t="s">
         <v>133</v>
       </c>
@@ -2602,7 +2695,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45.6">
+    <row r="6" spans="1:8" ht="47">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
@@ -2626,7 +2719,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45.6">
+    <row r="7" spans="1:8" ht="47">
       <c r="A7" s="14" t="s">
         <v>135</v>
       </c>
@@ -2650,7 +2743,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45.6">
+    <row r="8" spans="1:8" ht="47">
       <c r="A8" s="16" t="s">
         <v>126</v>
       </c>
@@ -2672,7 +2765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45.6">
+    <row r="9" spans="1:8" ht="47">
       <c r="A9" s="12" t="s">
         <v>128</v>
       </c>
@@ -2698,7 +2791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45.6">
+    <row r="10" spans="1:8" ht="47">
       <c r="A10" s="12" t="s">
         <v>129</v>
       </c>
@@ -2722,7 +2815,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45.6">
+    <row r="11" spans="1:8" ht="47">
       <c r="A11" s="12" t="s">
         <v>132</v>
       </c>
@@ -2746,7 +2839,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45.6">
+    <row r="12" spans="1:8" ht="47">
       <c r="A12" s="29" t="s">
         <v>147</v>
       </c>
@@ -2770,7 +2863,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45.6">
+    <row r="13" spans="1:8" ht="47">
       <c r="A13" s="29" t="s">
         <v>146</v>
       </c>
@@ -2792,7 +2885,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30.6">
+    <row r="14" spans="1:8" ht="31">
       <c r="A14" s="19" t="s">
         <v>130</v>
       </c>
@@ -2824,22 +2917,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45.6">
+    <row r="1" spans="1:6" ht="47">
       <c r="A1" s="39">
         <v>1</v>
       </c>
@@ -2859,7 +2952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45.6">
+    <row r="2" spans="1:6" ht="47">
       <c r="A2" s="39"/>
       <c r="B2" s="14" t="s">
         <v>135</v>
@@ -2877,7 +2970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45.6">
+    <row r="3" spans="1:6" ht="47">
       <c r="A3" s="39"/>
       <c r="B3" s="16" t="s">
         <v>125</v>
@@ -2895,7 +2988,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.6">
+    <row r="4" spans="1:6" ht="47">
       <c r="A4" s="39"/>
       <c r="B4" s="12" t="s">
         <v>132</v>
@@ -2913,8 +3006,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.95" customHeight="1"/>
-    <row r="6" spans="1:6" ht="45.6">
+    <row r="5" spans="1:6" ht="32" customHeight="1"/>
+    <row r="6" spans="1:6" ht="47">
       <c r="A6" s="41">
         <v>2</v>
       </c>
@@ -2934,7 +3027,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45.6">
+    <row r="7" spans="1:6" ht="47">
       <c r="A7" s="41"/>
       <c r="B7" s="12" t="s">
         <v>134</v>
@@ -2952,7 +3045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45.6">
+    <row r="8" spans="1:6" ht="47">
       <c r="A8" s="41"/>
       <c r="B8" s="12" t="s">
         <v>129</v>
@@ -2970,7 +3063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45.6">
+    <row r="9" spans="1:6" ht="47">
       <c r="A9" s="41"/>
       <c r="B9" s="16" t="s">
         <v>126</v>
@@ -2988,7 +3081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45.6">
+    <row r="10" spans="1:6" ht="47">
       <c r="A10" s="41"/>
       <c r="B10" s="29" t="s">
         <v>161</v>
@@ -3009,7 +3102,7 @@
     <row r="11" spans="1:6">
       <c r="F11" s="25"/>
     </row>
-    <row r="12" spans="1:6" ht="45.6">
+    <row r="12" spans="1:6" ht="47">
       <c r="A12" s="40">
         <v>3</v>
       </c>
@@ -3029,7 +3122,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45.6">
+    <row r="13" spans="1:6" ht="47">
       <c r="A13" s="40"/>
       <c r="B13" s="29" t="s">
         <v>147</v>
@@ -3047,7 +3140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45.6">
+    <row r="14" spans="1:6" ht="47">
       <c r="A14" s="40"/>
       <c r="B14" s="29" t="s">
         <v>146</v>
@@ -3065,7 +3158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45.6">
+    <row r="15" spans="1:6" ht="47">
       <c r="A15" s="40"/>
       <c r="B15" s="29" t="s">
         <v>160</v>
@@ -3096,19 +3189,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.95" customHeight="1">
+    <row r="1" spans="1:2" ht="32" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3140,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="62.4">
+    <row r="5" spans="1:2" ht="64">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>